<commit_message>
feat: add new ques
</commit_message>
<xml_diff>
--- a/00-记录统计.xlsx
+++ b/00-记录统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13240" tabRatio="688"/>
+    <workbookView windowWidth="30240" windowHeight="13360" tabRatio="688"/>
   </bookViews>
   <sheets>
     <sheet name="算法统计" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>题目</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>浮点数有很多易错点需要注意！！</t>
+  </si>
+  <si>
+    <t>code160-相交链表</t>
+  </si>
+  <si>
+    <t>2025.03.14</t>
   </si>
   <si>
     <t>内容</t>
@@ -1271,7 +1277,7 @@
   <dimension ref="A1:G229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
@@ -1558,11 +1564,21 @@
       <c r="G13" s="15"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="35" customHeight="1" spans="1:7">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="6">
+        <v>183</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="15"/>
     </row>
@@ -3522,10 +3538,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="35" customHeight="1" spans="1:3">
@@ -3533,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -3542,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6"/>
     </row>

</xml_diff>